<commit_message>
Added sampling display and CSV import to selection test app.
</commit_message>
<xml_diff>
--- a/SelectionTest/Data/PriceData.xlsx
+++ b/SelectionTest/Data/PriceData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SKU</t>
   </si>
@@ -37,6 +37,27 @@
   </si>
   <si>
     <t>Part 2</t>
+  </si>
+  <si>
+    <t>Part 3</t>
+  </si>
+  <si>
+    <t>Part 4</t>
+  </si>
+  <si>
+    <t>Part 5</t>
+  </si>
+  <si>
+    <t>Part 6</t>
+  </si>
+  <si>
+    <t>Part 7</t>
+  </si>
+  <si>
+    <t>Part 8</t>
+  </si>
+  <si>
+    <t>Part 9</t>
   </si>
 </sst>
 </file>
@@ -389,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +463,83 @@
         <v>42736</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>36387</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>5.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>

</xml_diff>